<commit_message>
Makeover last minute to release for testings
</commit_message>
<xml_diff>
--- a/dbs/data/activate/plantilla_de_activacion_V4.xlsx
+++ b/dbs/data/activate/plantilla_de_activacion_V4.xlsx
@@ -65,10 +65,10 @@
     <t xml:space="preserve">Teleinformatica</t>
   </si>
   <si>
-    <t xml:space="preserve">John Jairo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leuro</t>
+    <t xml:space="preserve">Scott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lang Ant</t>
   </si>
   <si>
     <t xml:space="preserve">C.C</t>
@@ -80,10 +80,10 @@
     <t xml:space="preserve">Logistica</t>
   </si>
   <si>
-    <t xml:space="preserve">Carolina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nose Los Apellidos</t>
+    <t xml:space="preserve">Harley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinn Daddy</t>
   </si>
   <si>
     <t xml:space="preserve">gabrielmasutier@gmail.com</t>
@@ -143,7 +143,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -212,6 +212,11 @@
       <name val="DejaVu Serif"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="DejaVu Serif"/>
+      <family val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -291,7 +296,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -340,11 +345,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,15 +365,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -554,7 +563,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3:F5"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -625,7 +634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" s="4" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -635,26 +644,26 @@
       <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="11" t="n">
         <v>85777666</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="14" t="n">
+      <c r="I4" s="15" t="n">
         <v>45753</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -664,22 +673,22 @@
       <c r="C5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="11" t="n">
         <v>35123123</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="14" t="n">
+      <c r="I5" s="15" t="n">
         <v>45753</v>
       </c>
     </row>
@@ -691,52 +700,52 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="14"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="14"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="14"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="14"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -765,122 +774,122 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="F3:F5 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="134.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="16" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="134.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="17" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="n">
+      <c r="A4" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="n">
+      <c r="A5" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="n">
+      <c r="A6" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="n">
+      <c r="A7" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="n">
+      <c r="A8" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="n">
+      <c r="A9" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="n">
+      <c r="A10" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="n">
+      <c r="A11" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="n">
+      <c r="A12" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="n">
+      <c r="A13" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="n">
+      <c r="A14" s="17" t="n">
         <v>11</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="n">
+      <c r="A15" s="17" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes in the login and the questionary
</commit_message>
<xml_diff>
--- a/dbs/data/activate/plantilla_de_activacion_V4.xlsx
+++ b/dbs/data/activate/plantilla_de_activacion_V4.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t xml:space="preserve">Formulario para inscripción de coordinaciones</t>
   </si>
@@ -98,19 +98,31 @@
     <t xml:space="preserve">Pregunta</t>
   </si>
   <si>
+    <t xml:space="preserve">CATEGORIAS</t>
+  </si>
+  <si>
     <t xml:space="preserve">El instructor acompaña y orienta la solución de sus dificultades académicas y personales.</t>
   </si>
   <si>
+    <t xml:space="preserve">NUNCA, DE VEZ EN CUANDO, SIEMPRE</t>
+  </si>
+  <si>
     <t xml:space="preserve">El instructor aplica estrategias participativas de trabajo en equipo que le permiten estar activo permanentemente en su proceso de aprendizaje.</t>
   </si>
   <si>
     <t xml:space="preserve">El instructor demuestra dominio técnico.</t>
   </si>
   <si>
+    <t xml:space="preserve">NO, SI</t>
+  </si>
+  <si>
     <t xml:space="preserve">El instructor desarrolla la totalidad de los resultados de aprendizaje programados.</t>
   </si>
   <si>
     <t xml:space="preserve">El instructor es puntual al iniciar las sesiones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUNCA, A VECES, SIEMPRE</t>
   </si>
   <si>
     <t xml:space="preserve">El instructor establece relaciones interpersonales cordiales, armoniosas y respetuosas.</t>
@@ -143,7 +155,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -212,11 +224,6 @@
       <name val="DejaVu Serif"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <name val="DejaVu Serif"/>
-      <family val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -345,7 +352,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,7 +360,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,7 +368,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,12 +376,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -560,10 +567,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -704,48 +711,37 @@
       <c r="I6" s="15"/>
     </row>
     <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="15"/>
-    </row>
-    <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -771,126 +767,166 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="134.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="17" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="153.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="40.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="16" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>24</v>
       </c>
+      <c r="C3" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="n">
+      <c r="A4" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>25</v>
+      <c r="B4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="n">
+      <c r="A5" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>26</v>
+      <c r="B5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="n">
+      <c r="A6" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="n">
+      <c r="A11" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>32</v>
+      <c r="B11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="n">
+      <c r="A12" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="n">
+      <c r="A13" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>34</v>
+      <c r="B13" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="n">
+      <c r="A14" s="16" t="n">
         <v>11</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>35</v>
+      <c r="B14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="n">
+      <c r="A15" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>36</v>
+      <c r="B15" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to original db name
</commit_message>
<xml_diff>
--- a/dbs/data/activate/plantilla_de_activacion_V4.xlsx
+++ b/dbs/data/activate/plantilla_de_activacion_V4.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
   <si>
     <t xml:space="preserve">Formulario para inscripción de coordinaciones</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">CGMT</t>
   </si>
   <si>
-    <t xml:space="preserve">Teleinformatica</t>
+    <t xml:space="preserve">INDUSTRIAS CREATIVAS</t>
   </si>
   <si>
     <t xml:space="preserve">Scott</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">masutier@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Logistica</t>
+    <t xml:space="preserve">LOGÍSTICA</t>
   </si>
   <si>
     <t xml:space="preserve">Harley</t>
@@ -87,6 +87,42 @@
   </si>
   <si>
     <t xml:space="preserve">gabrielmasutier@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERCADEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">littlescorpion@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELEINFORMÁTICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stryder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wanda@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSVERSAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ironman@test.com</t>
   </si>
   <si>
     <t xml:space="preserve">Preguntas de la evaluación</t>
@@ -150,12 +186,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -232,6 +269,17 @@
       <name val="DejaVu Serif"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="DejaVu Serif"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF0000FF"/>
+      <name val="DejaVu Serif"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -303,7 +351,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -352,6 +400,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,15 +420,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -570,7 +630,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -581,7 +641,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="28.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="10" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1019" style="1" width="11.53"/>
@@ -648,26 +708,26 @@
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="11" t="n">
         <v>85777666</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="15" t="n">
-        <v>45753</v>
+      <c r="I4" s="16" t="n">
+        <v>45782</v>
       </c>
     </row>
     <row r="5" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,71 +737,125 @@
       <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="11" t="n">
         <v>35123123</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="15" t="n">
-        <v>45753</v>
+      <c r="I5" s="16" t="n">
+        <v>45782</v>
       </c>
     </row>
     <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
+      <c r="A6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>95666222</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="16" t="n">
+        <v>45782</v>
+      </c>
     </row>
     <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="15"/>
+      <c r="A7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="13" t="n">
+        <v>75222444</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="16" t="n">
+        <v>45782</v>
+      </c>
     </row>
     <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="15"/>
+      <c r="A8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="13" t="n">
+        <v>79555777</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="16" t="n">
+        <v>45782</v>
+      </c>
     </row>
     <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="15"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -751,6 +865,9 @@
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" display="masutier@gmail.com"/>
     <hyperlink ref="H5" r:id="rId2" display="gabrielmasutier@gmail.com"/>
+    <hyperlink ref="H6" r:id="rId3" display="littlescorpion@test.com"/>
+    <hyperlink ref="H7" r:id="rId4" display="wanda@test.com"/>
+    <hyperlink ref="H8" r:id="rId5" display="ironman@test.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -775,158 +892,158 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="153.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="40.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="16" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="153.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="40.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="19" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>22</v>
+      <c r="A1" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>25</v>
+      <c r="A3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="n">
+      <c r="A4" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>27</v>
+      <c r="B4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="n">
+      <c r="A5" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>27</v>
+      <c r="B5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="n">
+      <c r="A6" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>30</v>
+      <c r="B6" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="n">
+      <c r="A7" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>30</v>
+      <c r="B7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="n">
+      <c r="A8" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>33</v>
+      <c r="B8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="n">
+      <c r="A9" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>33</v>
+      <c r="B9" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="n">
+      <c r="A10" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>27</v>
+      <c r="B10" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="n">
+      <c r="A11" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>33</v>
+      <c r="B11" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="n">
+      <c r="A12" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>33</v>
+      <c r="B12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="n">
+      <c r="A13" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>33</v>
+      <c r="B13" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="n">
+      <c r="A14" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>33</v>
+      <c r="B14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="n">
+      <c r="A15" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>33</v>
+      <c r="B15" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last testing ti'll preliminary testings
</commit_message>
<xml_diff>
--- a/dbs/data/activate/plantilla_de_activacion_V4.xlsx
+++ b/dbs/data/activate/plantilla_de_activacion_V4.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Coordinaciones" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Preguntas" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t xml:space="preserve">Formulario para inscripción de coordinaciones</t>
   </si>
@@ -59,70 +59,82 @@
     <t xml:space="preserve">Bogotá</t>
   </si>
   <si>
-    <t xml:space="preserve">CGMT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDUSTRIAS CREATIVAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scott</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lang Ant</t>
+    <t xml:space="preserve">CGMLTI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELEINFORMÁTICA E INDUSTRIAS CREATIVAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUSTAVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BELTRAN MACIAS</t>
   </si>
   <si>
     <t xml:space="preserve">C.C</t>
   </si>
   <si>
-    <t xml:space="preserve">masutier@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOGÍSTICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quinn Daddy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gabrielmasutier@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MERCADEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wednesday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">littlescorpion@test.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELEINFORMÁTICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stryder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wanda@test.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSVERSAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ironman@test.com</t>
+    <t xml:space="preserve">gbeltranm@sena.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOGÍSTICA Y FORMACIÓN COMPLEMENTARIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JHON JAIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEURO DELGADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jjleuro@sena.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERCADEO Y SEDES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIVIANA DEL MAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARANDA GUERRERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varanda@sena.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIRTUAL Y COMPLEMENTARIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHANY ANDRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASALINAS GOMEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jacasalinas@sena.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTICULACIÓN CON LA MEDIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANDREA YULIETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUENTES HERNANDEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apuentes@sena.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETAPA PRODUCTIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JULIAN ANDRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASTELLANOS CASTRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jacastellanos@sena.edu.co</t>
   </si>
   <si>
     <t xml:space="preserve">Preguntas de la evaluación</t>
@@ -137,49 +149,49 @@
     <t xml:space="preserve">CATEGORIAS</t>
   </si>
   <si>
-    <t xml:space="preserve">El instructor acompaña y orienta la solución de sus dificultades académicas y personales.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUNCA, DE VEZ EN CUANDO, SIEMPRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor aplica estrategias participativas de trabajo en equipo que le permiten estar activo permanentemente en su proceso de aprendizaje.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor demuestra dominio técnico.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO, SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor desarrolla la totalidad de los resultados de aprendizaje programados.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor es puntual al iniciar las sesiones.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUNCA, A VECES, SIEMPRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor establece relaciones interpersonales cordiales, armoniosas y respetuosas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor incentiva al aprendiz a utilizar la plataforma Territorium en el desarrollo de las actividades de aprendizaje.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor le da a conocer el proyecto formativo, la planeación pedagógica y las guiás de aprendizaje.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor le orienta su formación mediante un proyecto formativo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor le propone fuentes de consulta (Bibliografía,  Webgrafia...) y ayudas que facilitan su proceso de aprendizaje.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor revisa y asesora los planes de mejoramiento.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El instructor se preocupa por su mejoramiento continuo a nivel personal, social y laboral.</t>
+    <t xml:space="preserve">El instructor mantiene una actitud cordial y respetuosa al ingresar a la formación y a lo largo de todo el proceso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIEMPRE, CASI SIEMPRE, NUNCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor responde a mis inquietudes de manera respetuosa y utilizando un lenguaje comprensible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor crea un ambiente de confianza y respeto que me motiva a participar activamente en la formación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor promueve relaciones colaborativas en el marco del respeto mutuo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los temas abordados y las evidencias de aprendizaje asignadas fueron pertinentes y coherentes con la competencia desarrollada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor utiliza ejemplos prácticos, actividades interactivas y herramientas tecnológicas para facilitar mi aprendizaje.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor me presenta la guía de aprendizaje al inicio de cada fase de la formación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor promueve mi participación crítica y reflexiva.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor concerta el plan de trabajo de los resultados de aprendizaje al inicio de la formación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor demuestra disposición para reforzar explicaciones cuando lo requiera.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor brinda retroalimentación continua y permanente ayudando a mejorar mi aprendizaje.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor comunica de manera clara los criterios de evaluación para cada actividad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor evalúa y comunica los resultados de mis actividades a lo largo del proceso formativo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El instructor evalua resultado de aprendizaje según las fechas estrablecidas en el plan de trabajo.</t>
   </si>
 </sst>
 </file>
@@ -192,7 +204,7 @@
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -265,21 +277,25 @@
     <font>
       <u val="single"/>
       <sz val="10.5"/>
-      <color rgb="FF467886"/>
+      <color theme="10"/>
       <name val="DejaVu Serif"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <name val="DejaVu Serif"/>
-      <family val="1"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF0000FF"/>
       <name val="DejaVu Serif"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -294,16 +310,29 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -325,8 +354,15 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,8 +386,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -376,7 +415,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,10 +439,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -412,7 +447,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,11 +455,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,18 +471,23 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -486,7 +522,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
@@ -501,7 +537,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF467886"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -630,21 +666,20 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="28.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="10" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1019" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +696,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -711,23 +746,23 @@
       <c r="C4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="11" t="n">
-        <v>85777666</v>
-      </c>
-      <c r="H4" s="15" t="s">
+        <v>19423143</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="16" t="n">
-        <v>45782</v>
+      <c r="I4" s="15" t="n">
+        <v>45819</v>
       </c>
     </row>
     <row r="5" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,26 +775,26 @@
       <c r="C5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="11" t="n">
-        <v>35123123</v>
-      </c>
-      <c r="H5" s="15" t="s">
+        <v>79829839</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="16" t="n">
-        <v>45782</v>
-      </c>
-    </row>
-    <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5" s="15" t="n">
+        <v>45819</v>
+      </c>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
@@ -769,26 +804,26 @@
       <c r="C6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="11" t="n">
-        <v>95666222</v>
-      </c>
-      <c r="H6" s="18" t="s">
+        <v>1030623569</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="16" t="n">
-        <v>45782</v>
-      </c>
-    </row>
-    <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="15" t="n">
+        <v>45819</v>
+      </c>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
@@ -798,26 +833,26 @@
       <c r="C7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="13" t="n">
-        <v>75222444</v>
-      </c>
-      <c r="H7" s="18" t="s">
+      <c r="G7" s="12" t="n">
+        <v>80850368</v>
+      </c>
+      <c r="H7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="16" t="n">
-        <v>45782</v>
-      </c>
-    </row>
-    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="15" t="n">
+        <v>45819</v>
+      </c>
+    </row>
+    <row r="8" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
@@ -827,35 +862,53 @@
       <c r="C8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="13" t="n">
-        <v>79555777</v>
-      </c>
-      <c r="H8" s="18" t="s">
+      <c r="G8" s="12" t="n">
+        <v>52466223</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="16" t="n">
-        <v>45782</v>
-      </c>
-    </row>
-    <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="16"/>
+      <c r="I8" s="15" t="n">
+        <v>45819</v>
+      </c>
+    </row>
+    <row r="9" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>7181282</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="15" t="n">
+        <v>45819</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -863,11 +916,8 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" display="masutier@gmail.com"/>
-    <hyperlink ref="H5" r:id="rId2" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H6" r:id="rId3" display="littlescorpion@test.com"/>
-    <hyperlink ref="H7" r:id="rId4" display="wanda@test.com"/>
-    <hyperlink ref="H8" r:id="rId5" display="ironman@test.com"/>
+    <hyperlink ref="H4" r:id="rId1" display="gbeltranm@sena.edu.co"/>
+    <hyperlink ref="H9" r:id="rId2" display="jacastellanos@sena.edu.co"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -884,166 +934,188 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="153.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="40.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="19" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="153.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="40.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="17" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="n">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="n">
+      <c r="B4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="n">
+      <c r="B5" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="n">
+      <c r="B6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="n">
+      <c r="B7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="n">
+      <c r="B8" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="n">
+      <c r="B9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="n">
+      <c r="B10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="n">
+      <c r="B11" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="n">
+      <c r="B12" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="n">
+      <c r="B13" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="n">
         <v>11</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="n">
+      <c r="B14" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>45</v>
+      <c r="B15" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>